<commit_message>
update mostly on veg things
</commit_message>
<xml_diff>
--- a/data/raw_data/vegetation/241111_TEMPEST2_water_potentials.xlsx
+++ b/data/raw_data/vegetation/241111_TEMPEST2_water_potentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/peter_regier_pnnl_gov/Documents/Documents/GitHub/COMPASS-DOE/tempest2_do/data/raw_data/vegetation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1373" documentId="8_{D643C4A0-451E-184F-B9F1-0C02D3C5DFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEC67255-B0AA-B84C-A606-2258214973A1}"/>
+  <xr:revisionPtr revIDLastSave="1378" documentId="8_{D643C4A0-451E-184F-B9F1-0C02D3C5DFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{060B7135-76C3-B545-859A-26B7C5810525}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{DD320B44-C0DC-1A4D-8312-11C1ED59FF4A}"/>
   </bookViews>
@@ -209,10 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9031D31-7FEF-E44D-A258-C9AD138A55AA}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,7 +584,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45090</v>
       </c>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45090</v>
       </c>
@@ -630,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45090</v>
       </c>
@@ -653,7 +653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45090</v>
       </c>
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45090</v>
       </c>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45090</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45090</v>
       </c>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45090</v>
       </c>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45090</v>
       </c>
@@ -814,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45090</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45090</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45090</v>
       </c>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45090</v>
       </c>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45090</v>
       </c>
@@ -952,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45090</v>
       </c>
@@ -975,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45090</v>
       </c>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45090</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45090</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>45090</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>45090</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>45090</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45090</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>45090</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>45090</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>45090</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45090</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>45090</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>45090</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>45090</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45090</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45090</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45090</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45090</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45090</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45090</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45090</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45090</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45090</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45090</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45090</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45090</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45090</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45090</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45090</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45090</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45090</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45090</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>45090</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45090</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45090</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>45090</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>45090</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>45090</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>45090</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>45090</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>45090</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>45090</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>45090</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>45090</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>45090</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>45090</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>45090</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>45090</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>45090</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>45090</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>45090</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>45090</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>45090</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>45090</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>45090</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>45090</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>45090</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>45090</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>45090</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>45090</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>45090</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>45090</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>45090</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>45090</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>45090</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>45090</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>45090</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>45090</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>45090</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>45090</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>45090</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>45090</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>45090</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>45090</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>45090</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>45090</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>45090</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>45090</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>45090</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>45090</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>45090</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>45090</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>45090</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>45090</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>45090</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>45090</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>45090</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>45090</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>45090</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>45090</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>45090</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>45090</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>45090</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>45090</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>45090</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>45090</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>45090</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>45090</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>45090</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>45090</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>45090</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>45090</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>45090</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>45090</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>45090</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>45090</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>45090</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>45090</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>45090</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>45090</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>45090</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>45090</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>45090</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>45090</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>45090</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>45090</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>45090</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>45090</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>45090</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>45090</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>45090</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>45090</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>45090</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>45090</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>45090</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>45090</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>45090</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>45090</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>45090</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>45090</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>45090</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>45090</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>45090</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>45090</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>45090</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>45090</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>45090</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>45090</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>45090</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>45090</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>45090</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>45090</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>45090</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>45090</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>45090</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>45090</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>45090</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>45090</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>45090</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>45090</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>45090</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>45090</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>45090</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>45090</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>45090</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>45090</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>45090</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>45090</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>45090</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>45090</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>45090</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>45090</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>45090</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>45090</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>45090</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>45090</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>45090</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>45090</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>45090</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>45090</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>45090</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>45090</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>45090</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>45090</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>45090</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>45090</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>45090</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>45090</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>45090</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>45090</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>45090</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>45090</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>45090</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>45090</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>45090</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>45090</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>45090</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>45090</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>45090</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>45090</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>45090</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>45090</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>45090</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>45090</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>45090</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>45090</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>45090</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>45090</v>
       </c>
@@ -5590,7 +5590,7 @@
       <c r="D229">
         <v>35</v>
       </c>
-      <c r="E229" s="2">
+      <c r="E229">
         <v>1229</v>
       </c>
       <c r="F229">
@@ -5600,7 +5600,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>45090</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>45090</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>45090</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>45090</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>45090</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>45090</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>45090</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>45090</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>45090</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>45090</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>45090</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>45090</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>45090</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>45090</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>45090</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>45090</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>45090</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>45090</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>45090</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>45090</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>45090</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>45090</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>45090</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>45090</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>54</v>
       </c>
       <c r="E253">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F253">
         <v>1.1499999999999999</v>
@@ -6149,7 +6149,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>45090</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>55</v>
       </c>
       <c r="E254">
-        <v>302</v>
+        <v>1502</v>
       </c>
       <c r="G254" t="s">
         <v>36</v>
@@ -6172,7 +6172,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>45090</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>45090</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>45090</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>45090</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>45090</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>45090</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>45090</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>45090</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>45090</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>45090</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>45090</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>45090</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>45090</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>45090</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>45090</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>45090</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>45090</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>45090</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>45090</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>45090</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>45090</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>45090</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>45090</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>45090</v>
       </c>
@@ -6724,7 +6724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>45090</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>45090</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>45090</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>45090</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>45090</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>45090</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>45090</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>45090</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>45090</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>45090</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>45090</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>45090</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>45090</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>45090</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>45090</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>45090</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>45090</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>45090</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>45090</v>
       </c>
@@ -7162,6 +7162,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C297" xr:uid="{D9031D31-7FEF-E44D-A258-C9AD138A55AA}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="F13"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>